<commit_message>
update listener and data
</commit_message>
<xml_diff>
--- a/AASProductTestTools/src/main/java/AASProductTestCase/AASProductTest/qa/testdata/ExtraPTPositiveData.xlsx
+++ b/AASProductTestTools/src/main/java/AASProductTestCase/AASProductTest/qa/testdata/ExtraPTPositiveData.xlsx
@@ -411,7 +411,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -422,7 +422,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -433,7 +433,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -444,7 +444,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -455,7 +455,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -466,7 +466,7 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -477,7 +477,7 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -488,7 +488,7 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -499,7 +499,7 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -510,7 +510,7 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -521,7 +521,7 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -532,7 +532,7 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -543,7 +543,7 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -554,7 +554,7 @@
         <v>14</v>
       </c>
       <c r="C15">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for new extent report
</commit_message>
<xml_diff>
--- a/AASProductTestTools/src/main/java/AASProductTestCase/AASProductTest/qa/testdata/ExtraPTPositiveData.xlsx
+++ b/AASProductTestTools/src/main/java/AASProductTestCase/AASProductTest/qa/testdata/ExtraPTPositiveData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="5364"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12792" windowHeight="5076"/>
   </bookViews>
   <sheets>
     <sheet name="PositiveExtra" sheetId="1" r:id="rId1"/>
@@ -15,18 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="4">
-  <si>
-    <t>AG</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>ProdID</t>
   </si>
   <si>
     <t>PT</t>
-  </si>
-  <si>
-    <t>PIKACHU</t>
   </si>
 </sst>
 </file>
@@ -386,8 +380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -399,161 +393,116 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B3">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>3</v>
-      </c>
-      <c r="C4">
+      <c r="B4">
         <v>10.5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="C5">
+      <c r="B5">
         <v>10.5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="C6">
+      <c r="B6">
         <v>10.5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="B7">
         <v>10.5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="2">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="C8">
+      <c r="B8">
         <v>10.5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="C9">
+      <c r="B9">
         <v>10.5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="2">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="C10">
+      <c r="B10">
         <v>10.5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="2">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="C11">
+      <c r="B11">
         <v>10.5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="2">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="C12">
+      <c r="B12">
         <v>10.5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="2">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="C13">
+      <c r="B13">
         <v>10.5</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="2">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="C14">
+      <c r="B14">
         <v>10.5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="2">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="C15">
+      <c r="B15">
         <v>10.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Complete Custom Extent
</commit_message>
<xml_diff>
--- a/AASProductTestTools/src/main/java/AASProductTestCase/AASProductTest/qa/testdata/ExtraPTPositiveData.xlsx
+++ b/AASProductTestTools/src/main/java/AASProductTestCase/AASProductTest/qa/testdata/ExtraPTPositiveData.xlsx
@@ -380,8 +380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -399,7 +399,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -407,7 +407,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -415,7 +415,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -423,7 +423,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -431,7 +431,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -439,7 +439,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -447,7 +447,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -455,7 +455,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -463,7 +463,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -471,7 +471,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -479,7 +479,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -487,7 +487,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -495,7 +495,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -503,7 +503,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update For Skin Test
</commit_message>
<xml_diff>
--- a/AASProductTestTools/src/main/java/AASProductTestCase/AASProductTest/qa/testdata/ExtraPTPositiveData.xlsx
+++ b/AASProductTestTools/src/main/java/AASProductTestCase/AASProductTest/qa/testdata/ExtraPTPositiveData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12792" windowHeight="5076"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12792" windowHeight="5064"/>
   </bookViews>
   <sheets>
     <sheet name="PositiveExtra" sheetId="1" r:id="rId1"/>
@@ -399,7 +399,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>11.5</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -407,7 +407,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>11.5</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -415,7 +415,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>11.5</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -423,7 +423,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>11.5</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -431,7 +431,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>11.5</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -439,7 +439,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>11.5</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -447,7 +447,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>11.5</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -455,7 +455,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>11.5</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -463,7 +463,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>11.5</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -471,7 +471,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>11.5</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -479,7 +479,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>11.5</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -487,7 +487,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>11.5</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -495,7 +495,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>11.5</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -503,7 +503,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>11.5</v>
+        <v>13.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Product Setting Test Update
</commit_message>
<xml_diff>
--- a/AASProductTestTools/src/main/java/AASProductTestCase/AASProductTest/qa/testdata/ExtraPTPositiveData.xlsx
+++ b/AASProductTestTools/src/main/java/AASProductTestCase/AASProductTest/qa/testdata/ExtraPTPositiveData.xlsx
@@ -4,23 +4,69 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12792" windowHeight="5064"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12792" windowHeight="5160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PositiveExtra" sheetId="1" r:id="rId1"/>
+    <sheet name="ProductList" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:L16"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>ProdID</t>
   </si>
   <si>
     <t>PT</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Evolution</t>
+  </si>
+  <si>
+    <t>Paiza</t>
+  </si>
+  <si>
+    <t>Pragmatic Slot</t>
+  </si>
+  <si>
+    <t>Habanero Slot</t>
+  </si>
+  <si>
+    <t>Maverick Slot</t>
+  </si>
+  <si>
+    <t>Netent Slot</t>
+  </si>
+  <si>
+    <t>Quicksipn Slot</t>
+  </si>
+  <si>
+    <t>Spade Gaming Slot</t>
+  </si>
+  <si>
+    <t>Big Gaming</t>
+  </si>
+  <si>
+    <t>Micro Gaming</t>
+  </si>
+  <si>
+    <t>Asia Gaming</t>
+  </si>
+  <si>
+    <t>Dream Gaming</t>
+  </si>
+  <si>
+    <t>Praagmatic Gaming</t>
+  </si>
+  <si>
+    <t>Sexy Gaming</t>
   </si>
 </sst>
 </file>
@@ -380,8 +426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B15"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,4 +556,142 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update for product setting test
</commit_message>
<xml_diff>
--- a/AASProductTestTools/src/main/java/AASProductTestCase/AASProductTest/qa/testdata/ExtraPTPositiveData.xlsx
+++ b/AASProductTestTools/src/main/java/AASProductTestCase/AASProductTest/qa/testdata/ExtraPTPositiveData.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12792" windowHeight="5160" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12792" windowHeight="3756"/>
   </bookViews>
   <sheets>
     <sheet name="PositiveExtra" sheetId="1" r:id="rId1"/>
     <sheet name="ProductList" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:L16"/>
+  <oleSize ref="A5:M15"/>
 </workbook>
 </file>
 
@@ -426,7 +426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A15"/>
     </sheetView>
   </sheetViews>
@@ -562,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update for Report node structure
</commit_message>
<xml_diff>
--- a/AASProductTestTools/src/main/java/AASProductTestCase/AASProductTest/qa/testdata/ExtraPTPositiveData.xlsx
+++ b/AASProductTestTools/src/main/java/AASProductTestCase/AASProductTest/qa/testdata/ExtraPTPositiveData.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12792" windowHeight="3756"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12792" windowHeight="4848" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PositiveExtra" sheetId="1" r:id="rId1"/>
     <sheet name="ProductList" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A5:M15"/>
+  <oleSize ref="A7:L21"/>
 </workbook>
 </file>
 
@@ -426,8 +426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -445,7 +445,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>13.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -453,7 +453,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>13.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -461,7 +461,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>13.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -469,7 +469,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>13.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -477,7 +477,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>13.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -485,7 +485,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>13.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -493,7 +493,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>13.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -501,7 +501,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>13.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -509,7 +509,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>13.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -517,7 +517,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>13.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -525,7 +525,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>13.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -533,7 +533,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>13.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -541,7 +541,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>13.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -549,7 +549,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>13.5</v>
+        <v>10.5</v>
       </c>
     </row>
   </sheetData>
@@ -562,7 +562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update For PT Setting
</commit_message>
<xml_diff>
--- a/AASProductTestTools/src/main/java/AASProductTestCase/AASProductTest/qa/testdata/ExtraPTPositiveData.xlsx
+++ b/AASProductTestTools/src/main/java/AASProductTestCase/AASProductTest/qa/testdata/ExtraPTPositiveData.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12792" windowHeight="4848" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12792" windowHeight="4908"/>
   </bookViews>
   <sheets>
     <sheet name="PositiveExtra" sheetId="1" r:id="rId1"/>
     <sheet name="ProductList" sheetId="2" r:id="rId2"/>
+    <sheet name="CAPTSetting" sheetId="3" r:id="rId3"/>
+    <sheet name="SMAPTSetting" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A7:L21"/>
+  <oleSize ref="A1:M15"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="21">
   <si>
     <t>ProdID</t>
   </si>
@@ -67,6 +69,18 @@
   </si>
   <si>
     <t>Sexy Gaming</t>
+  </si>
+  <si>
+    <t>PPT1</t>
+  </si>
+  <si>
+    <t>Play n Go</t>
+  </si>
+  <si>
+    <t>NPT1</t>
+  </si>
+  <si>
+    <t>NPT2</t>
   </si>
 </sst>
 </file>
@@ -424,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,6 +563,14 @@
         <v>14</v>
       </c>
       <c r="B15">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16">
         <v>10.5</v>
       </c>
     </row>
@@ -560,10 +582,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -691,6 +713,594 @@
         <v>10</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>50.5</v>
+      </c>
+      <c r="D2">
+        <v>49</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>50.5</v>
+      </c>
+      <c r="D3">
+        <v>49</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>50.5</v>
+      </c>
+      <c r="D4">
+        <v>49</v>
+      </c>
+      <c r="E4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>50.5</v>
+      </c>
+      <c r="D5">
+        <v>49</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>50.5</v>
+      </c>
+      <c r="D6">
+        <v>49</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>50.5</v>
+      </c>
+      <c r="D7">
+        <v>49</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>50.5</v>
+      </c>
+      <c r="D8">
+        <v>49</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>50.5</v>
+      </c>
+      <c r="D9">
+        <v>49</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>50.5</v>
+      </c>
+      <c r="D10">
+        <v>49</v>
+      </c>
+      <c r="E10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>50.5</v>
+      </c>
+      <c r="D11">
+        <v>49</v>
+      </c>
+      <c r="E11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>50.5</v>
+      </c>
+      <c r="D12">
+        <v>49</v>
+      </c>
+      <c r="E12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>50.5</v>
+      </c>
+      <c r="D13">
+        <v>49</v>
+      </c>
+      <c r="E13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>50.5</v>
+      </c>
+      <c r="D14">
+        <v>49</v>
+      </c>
+      <c r="E14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>50.5</v>
+      </c>
+      <c r="D15">
+        <v>49</v>
+      </c>
+      <c r="E15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16">
+        <v>50.5</v>
+      </c>
+      <c r="D16">
+        <v>49</v>
+      </c>
+      <c r="E16">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>19</v>
+      </c>
+      <c r="E2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>19</v>
+      </c>
+      <c r="E4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>19</v>
+      </c>
+      <c r="E5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>19</v>
+      </c>
+      <c r="E6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>19</v>
+      </c>
+      <c r="E7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>19</v>
+      </c>
+      <c r="E8">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>19</v>
+      </c>
+      <c r="E9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <v>19</v>
+      </c>
+      <c r="E10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>20</v>
+      </c>
+      <c r="D11">
+        <v>19</v>
+      </c>
+      <c r="E11">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <v>19</v>
+      </c>
+      <c r="E12">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>20</v>
+      </c>
+      <c r="D13">
+        <v>19</v>
+      </c>
+      <c r="E13">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>20</v>
+      </c>
+      <c r="D14">
+        <v>19</v>
+      </c>
+      <c r="E14">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>20</v>
+      </c>
+      <c r="D15">
+        <v>19</v>
+      </c>
+      <c r="E15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16">
+        <v>20</v>
+      </c>
+      <c r="D16">
+        <v>19</v>
+      </c>
+      <c r="E16">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update for PT Setting Fix
</commit_message>
<xml_diff>
--- a/AASProductTestTools/src/main/java/AASProductTestCase/AASProductTest/qa/testdata/ExtraPTPositiveData.xlsx
+++ b/AASProductTestTools/src/main/java/AASProductTestCase/AASProductTest/qa/testdata/ExtraPTPositiveData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12792" windowHeight="4908"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12792" windowHeight="4908" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PositiveExtra" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="SMAPTSetting" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M15"/>
+  <oleSize ref="A7:L21"/>
 </workbook>
 </file>
 
@@ -440,8 +440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,7 +459,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>10.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -467,7 +467,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>10.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -475,7 +475,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>10.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -483,7 +483,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>10.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -491,7 +491,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>10.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -499,7 +499,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>10.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -507,7 +507,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>10.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -515,7 +515,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>10.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -523,7 +523,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>10.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -531,7 +531,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>10.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -539,7 +539,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>10.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -547,7 +547,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>10.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -555,7 +555,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>10.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -563,7 +563,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>10.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -571,7 +571,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>10.5</v>
+        <v>12.5</v>
       </c>
     </row>
   </sheetData>
@@ -584,7 +584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A16" sqref="A16:B16"/>
     </sheetView>
   </sheetViews>
@@ -730,7 +730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1020,7 +1020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update for new product
</commit_message>
<xml_diff>
--- a/AASProductTestTools/src/main/java/AASProductTestCase/AASProductTest/qa/testdata/ExtraPTPositiveData.xlsx
+++ b/AASProductTestTools/src/main/java/AASProductTestCase/AASProductTest/qa/testdata/ExtraPTPositiveData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12792" windowHeight="4908" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12792" windowHeight="4908" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PositiveExtra" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,12 @@
     <sheet name="SMAPTSetting" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A7:L21"/>
+  <oleSize ref="A8:L22"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="23">
   <si>
     <t>ProdID</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>NPT2</t>
+  </si>
+  <si>
+    <t>World Match</t>
+  </si>
+  <si>
+    <t>Inplay Matrix</t>
   </si>
 </sst>
 </file>
@@ -582,10 +588,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:B16"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -721,6 +727,22 @@
         <v>18</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -728,10 +750,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1011,6 +1033,40 @@
         <v>100</v>
       </c>
     </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>50.5</v>
+      </c>
+      <c r="D17">
+        <v>49</v>
+      </c>
+      <c r="E17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18">
+        <v>50.5</v>
+      </c>
+      <c r="D18">
+        <v>49</v>
+      </c>
+      <c r="E18">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1018,10 +1074,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1301,6 +1357,40 @@
         <v>80</v>
       </c>
     </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>20</v>
+      </c>
+      <c r="D17">
+        <v>19</v>
+      </c>
+      <c r="E17">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18">
+        <v>20</v>
+      </c>
+      <c r="D18">
+        <v>19</v>
+      </c>
+      <c r="E18">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update new product on PT Setting
</commit_message>
<xml_diff>
--- a/AASProductTestTools/src/main/java/AASProductTestCase/AASProductTest/qa/testdata/ExtraPTPositiveData.xlsx
+++ b/AASProductTestTools/src/main/java/AASProductTestCase/AASProductTest/qa/testdata/ExtraPTPositiveData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12792" windowHeight="4908" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12792" windowHeight="4860" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PositiveExtra" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="SMAPTSetting" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A8:L22"/>
+  <oleSize ref="A1:L15"/>
 </workbook>
 </file>
 
@@ -444,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B16"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -577,6 +577,22 @@
         <v>15</v>
       </c>
       <c r="B16">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18">
         <v>12.5</v>
       </c>
     </row>
@@ -588,10 +604,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:B18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -599,7 +615,7 @@
     <col min="2" max="2" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -607,7 +623,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -615,7 +631,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -623,7 +639,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -631,7 +647,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -639,7 +655,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -647,7 +663,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -655,23 +671,23 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -679,7 +695,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -687,7 +703,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -695,7 +711,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -703,7 +719,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -711,7 +727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -719,7 +735,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -745,6 +761,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -752,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:B18"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1076,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update for UK24 Prod Setting
</commit_message>
<xml_diff>
--- a/AASProductTestTools/src/main/java/AASProductTestCase/AASProductTest/qa/testdata/ExtraPTPositiveData.xlsx
+++ b/AASProductTestTools/src/main/java/AASProductTestCase/AASProductTest/qa/testdata/ExtraPTPositiveData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12792" windowHeight="4860"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13068" windowHeight="4596" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PositiveExtra" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,12 @@
     <sheet name="SMAPTSetting" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A8:M22"/>
+  <oleSize ref="A8:L21"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="25">
   <si>
     <t>ProdID</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Pragmatic Gaming</t>
+  </si>
+  <si>
+    <t>UK24</t>
   </si>
 </sst>
 </file>
@@ -447,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -596,6 +599,14 @@
         <v>17</v>
       </c>
       <c r="B18">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19">
         <v>12.5</v>
       </c>
     </row>
@@ -607,10 +618,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -762,6 +773,14 @@
         <v>22</v>
       </c>
     </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -770,10 +789,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C19" sqref="C19:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1087,6 +1106,23 @@
         <v>100</v>
       </c>
     </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19">
+        <v>50.5</v>
+      </c>
+      <c r="D19">
+        <v>49</v>
+      </c>
+      <c r="E19">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1094,10 +1130,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1411,6 +1447,23 @@
         <v>80</v>
       </c>
     </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19">
+        <v>20</v>
+      </c>
+      <c r="D19">
+        <v>19</v>
+      </c>
+      <c r="E19">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>